<commit_message>
17th Commit - Scanning Operational
Sucessfully got the scanner to take pictures and process data using the Ras-Pi and Arducam. Unsure if extacted data is good yet, need to run actual test with the laser line.
</commit_message>
<xml_diff>
--- a/3D_Scan/Matrices.xlsx
+++ b/3D_Scan/Matrices.xlsx
@@ -371,28 +371,28 @@
         <v>0</v>
       </c>
       <c r="H1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J1">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="K1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="L1">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="M1">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="N1">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="O1">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="P1">
         <v>0</v>
@@ -464,19 +464,19 @@
         <v>0</v>
       </c>
       <c r="AM1">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="AN1">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="AO1">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="AP1">
         <v>0</v>
       </c>
       <c r="AQ1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR1">
         <v>0</v>
@@ -485,10 +485,10 @@
         <v>0</v>
       </c>
       <c r="AT1">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AU1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AV1">
         <v>0</v>
@@ -523,25 +523,25 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -672,19 +672,19 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="X3">
-        <v>416</v>
+        <v>0</v>
       </c>
       <c r="Y3">
         <v>0</v>
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="AK3">
-        <v>215</v>
+        <v>0</v>
       </c>
       <c r="AL3">
         <v>0</v>
@@ -759,31 +759,31 @@
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>452</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>451</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>446</v>
+        <v>0</v>
       </c>
       <c r="AQ3">
-        <v>451</v>
+        <v>0</v>
       </c>
       <c r="AR3">
-        <v>438</v>
+        <v>0</v>
       </c>
       <c r="AS3">
-        <v>433</v>
+        <v>0</v>
       </c>
       <c r="AT3">
-        <v>431</v>
+        <v>0</v>
       </c>
       <c r="AU3">
-        <v>420</v>
+        <v>0</v>
       </c>
       <c r="AV3">
-        <v>344</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>